<commit_message>
cierre de proyecto comparape
</commit_message>
<xml_diff>
--- a/Linea Base/comparape/lb1/SCPPN_CP.xlsx
+++ b/Linea Base/comparape/lb1/SCPPN_CP.xlsx
@@ -122,12 +122,6 @@
     <t xml:space="preserve">Elaboracion de Pruebas Unitarias </t>
   </si>
   <si>
-    <t>Elaboracion de Pruebas de stress</t>
-  </si>
-  <si>
-    <t>Elaboracion de Plan de pruebas</t>
-  </si>
-  <si>
     <t>Hito #5: Pruebas 08-01-2021</t>
   </si>
   <si>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>Fecha de Inicio: 21/10/2020</t>
+  </si>
+  <si>
+    <t>Elaboracion de Pruebas de carga</t>
+  </si>
+  <si>
+    <t>Elaboracion de plan de pruebas</t>
   </si>
 </sst>
 </file>
@@ -188,13 +188,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,12 +205,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCFE2F3"/>
         <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -339,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,53 +386,34 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -664,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -687,34 +662,34 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
+      <c r="B3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
+      <c r="B4" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -745,7 +720,7 @@
         <v>44125</v>
       </c>
       <c r="D6" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="10">
         <v>44128</v>
@@ -766,7 +741,7 @@
         <v>44125</v>
       </c>
       <c r="D7" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="10">
         <v>44125</v>
@@ -813,200 +788,199 @@
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="34">
+      <c r="C10" s="24">
         <v>44193</v>
       </c>
-      <c r="D10" s="35">
+      <c r="D10" s="25">
+        <v>2</v>
+      </c>
+      <c r="E10" s="24">
+        <v>44194</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="26">
         <v>1</v>
       </c>
-      <c r="E10" s="34">
-        <v>44194</v>
-      </c>
-      <c r="F10" s="35" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="22"/>
+    </row>
+    <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="24">
+        <v>44195</v>
+      </c>
+      <c r="D11" s="25">
+        <v>1</v>
+      </c>
+      <c r="E11" s="24">
+        <v>44195</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="26">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="22"/>
+    </row>
+    <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B12" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="29">
+        <v>44193</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="29">
+        <v>44195</v>
+      </c>
+      <c r="F12" s="25"/>
+      <c r="G12" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" s="34" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B13" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="24">
+        <v>44195</v>
+      </c>
+      <c r="D13" s="25">
+        <v>1</v>
+      </c>
+      <c r="E13" s="24">
+        <v>44195</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="24">
+        <v>44196</v>
+      </c>
+      <c r="D14" s="25">
+        <v>2</v>
+      </c>
+      <c r="E14" s="31">
+        <v>44197</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="26">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="24">
+        <v>44196</v>
+      </c>
+      <c r="D15" s="25">
+        <v>2</v>
+      </c>
+      <c r="E15" s="31">
+        <v>44197</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G15" s="26">
         <v>1</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="27"/>
-    </row>
-    <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="34">
-        <v>44195</v>
-      </c>
-      <c r="D11" s="35">
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B16" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="31">
+        <v>44197</v>
+      </c>
+      <c r="D16" s="25">
+        <v>2</v>
+      </c>
+      <c r="E16" s="31">
+        <v>44198</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="26">
         <v>1</v>
       </c>
-      <c r="E11" s="34">
-        <v>44195</v>
-      </c>
-      <c r="F11" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="36">
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="29">
+        <v>44196</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="29">
+        <v>44198</v>
+      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26">
         <v>1</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="27"/>
-    </row>
-    <row r="12" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="39">
-        <v>44193</v>
-      </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="39">
-        <v>44195</v>
-      </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="34">
-        <v>44196</v>
-      </c>
-      <c r="D13" s="35">
-        <v>5</v>
-      </c>
-      <c r="E13" s="41">
-        <v>44197</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="36">
-        <v>1</v>
-      </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="34">
-        <v>44196</v>
-      </c>
-      <c r="D14" s="35">
-        <v>5</v>
-      </c>
-      <c r="E14" s="41">
-        <v>44197</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="36">
-        <v>1</v>
-      </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="41">
-        <v>44197</v>
-      </c>
-      <c r="D15" s="35">
+    </row>
+    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="31">
+        <v>44199</v>
+      </c>
+      <c r="D18" s="25">
         <v>3</v>
       </c>
-      <c r="E15" s="41">
-        <v>44198</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="36">
-        <v>1</v>
-      </c>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="34">
-        <v>44195</v>
-      </c>
-      <c r="D16" s="35">
-        <v>1</v>
-      </c>
-      <c r="E16" s="34">
-        <v>44195</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="36">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="39">
-        <v>44196</v>
-      </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="39">
-        <v>44198</v>
-      </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="30">
-        <v>44199</v>
-      </c>
-      <c r="D18" s="25">
-        <v>4</v>
-      </c>
-      <c r="E18" s="30">
-        <v>44200</v>
+      <c r="E18" s="31">
+        <v>44201</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>25</v>
       </c>
       <c r="G18" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="31">
         <v>44199</v>
       </c>
       <c r="D19" s="25">
-        <v>24</v>
-      </c>
-      <c r="E19" s="30">
+        <v>1</v>
+      </c>
+      <c r="E19" s="31">
         <v>44200</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="26">
@@ -1015,19 +989,19 @@
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="31">
         <v>44200</v>
       </c>
       <c r="D20" s="25">
-        <v>24</v>
-      </c>
-      <c r="E20" s="30">
+        <v>2</v>
+      </c>
+      <c r="E20" s="31">
         <v>44201</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="25" t="s">
         <v>20</v>
       </c>
       <c r="G20" s="26">
@@ -1036,44 +1010,44 @@
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="31">
         <v>44200</v>
       </c>
       <c r="D21" s="25">
-        <v>24</v>
-      </c>
-      <c r="E21" s="30">
-        <v>44200</v>
+        <v>2</v>
+      </c>
+      <c r="E21" s="31">
+        <v>44201</v>
       </c>
       <c r="F21" s="25" t="s">
         <v>25</v>
       </c>
       <c r="G21" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="31">
         <v>44201</v>
       </c>
       <c r="D22" s="25">
-        <v>24</v>
-      </c>
-      <c r="E22" s="30">
+        <v>1</v>
+      </c>
+      <c r="E22" s="31">
         <v>44201</v>
       </c>
       <c r="F22" s="25" t="s">
         <v>25</v>
       </c>
       <c r="G22" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="3"/>
     </row>
@@ -1090,75 +1064,75 @@
       </c>
       <c r="F23" s="25"/>
       <c r="G23" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="30">
-        <v>44199</v>
-      </c>
-      <c r="D24" s="24">
+      <c r="C24" s="31">
+        <v>44202</v>
+      </c>
+      <c r="D24" s="25">
         <v>1</v>
       </c>
-      <c r="E24" s="30">
-        <v>44199</v>
+      <c r="E24" s="31">
+        <v>44202</v>
       </c>
       <c r="F24" s="25" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="30">
-        <v>44200</v>
-      </c>
-      <c r="D25" s="24">
+      <c r="B25" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="31">
+        <v>44203</v>
+      </c>
+      <c r="D25" s="25">
         <v>1</v>
       </c>
-      <c r="E25" s="30">
-        <v>44200</v>
+      <c r="E25" s="31">
+        <v>44203</v>
       </c>
       <c r="F25" s="25" t="s">
         <v>22</v>
       </c>
       <c r="G25" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="23">
+      <c r="B26" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="31">
         <v>44204</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="25">
         <v>1</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="31">
         <v>44204</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="25" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" s="29">
         <v>44202</v>
@@ -1168,7 +1142,9 @@
         <v>44204</v>
       </c>
       <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="G27" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
@@ -7967,6 +7943,6 @@
     <mergeCell ref="B4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>